<commit_message>
changes added 298331 to intsus
</commit_message>
<xml_diff>
--- a/templates/template_loans_ifrs.xlsx
+++ b/templates/template_loans_ifrs.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8328"/>
   </bookViews>
   <sheets>
     <sheet name="Export Worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Export Worksheet'!$A$5:$W$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Export Worksheet'!$A$5:$X$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -28,7 +28,7 @@
     <author>Bruce Higiro Munyandamutsa</author>
   </authors>
   <commentList>
-    <comment ref="S6" authorId="0" shapeId="0">
+    <comment ref="T6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T6" authorId="0" shapeId="0">
+    <comment ref="U6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>BRANCH</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>PROV_INT</t>
+  </si>
+  <si>
+    <t>AGIOS_CDT_MARCH</t>
   </si>
 </sst>
 </file>
@@ -342,11 +345,11 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +657,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,45 +679,45 @@
     <col min="12" max="12" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.44140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="8" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" style="8" customWidth="1"/>
+    <col min="15" max="16" width="14.88671875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.44140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12" style="7" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="6.109375" style="7" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="H4" s="4">
         <f>SUM(H5:H20000)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:O4" si="0">SUM(I5:I20000)</f>
+        <f t="shared" ref="I4:P4" si="0">SUM(I5:I20000)</f>
         <v>0</v>
       </c>
       <c r="J4" s="4">
@@ -741,8 +744,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="P4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -789,42 +796,45 @@
         <v>24</v>
       </c>
       <c r="P5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="X5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="Y5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="S6" s="3" t="str">
-        <f>IFERROR(DATE(RIGHT(Y6,4),MID(Y6,4,2),LEFT(Y6,2)),"")</f>
-        <v/>
-      </c>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T6" s="3" t="str">
         <f>IFERROR(DATE(RIGHT(Z6,4),MID(Z6,4,2),LEFT(Z6,2)),"")</f>
+        <v/>
+      </c>
+      <c r="U6" s="3" t="str">
+        <f>IFERROR(DATE(RIGHT(AA6,4),MID(AA6,4,2),LEFT(AA6,2)),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>